<commit_message>
Updating now that Moscow worked
</commit_message>
<xml_diff>
--- a/3-Unpack/how-I-parse-the-xml.xlsx
+++ b/3-Unpack/how-I-parse-the-xml.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="88">
   <si>
     <t>OutputTable</t>
   </si>
@@ -224,6 +224,60 @@
   </si>
   <si>
     <t>/*/d1:contract/oos:finances/oos:budget/oos:name</t>
+  </si>
+  <si>
+    <t>XMLFieldName</t>
+  </si>
+  <si>
+    <t>oos:id</t>
+  </si>
+  <si>
+    <t>oos:regNum</t>
+  </si>
+  <si>
+    <t>oos:publishDate</t>
+  </si>
+  <si>
+    <t>oos:signDate</t>
+  </si>
+  <si>
+    <t>oos:versionNumber</t>
+  </si>
+  <si>
+    <t>oos:price</t>
+  </si>
+  <si>
+    <t>oos:customer/oos:regNum</t>
+  </si>
+  <si>
+    <t>oos:customer/oos:fullName</t>
+  </si>
+  <si>
+    <t>oos:customer/oos:inn</t>
+  </si>
+  <si>
+    <t>oos:customer/oos:kpp</t>
+  </si>
+  <si>
+    <t>oos:customer/oos:tofk</t>
+  </si>
+  <si>
+    <t>oos:currency/oos:code</t>
+  </si>
+  <si>
+    <t>oos:execution/oos:month</t>
+  </si>
+  <si>
+    <t>oos:execution/oos:year</t>
+  </si>
+  <si>
+    <t>oos:finances/oos:financeSource</t>
+  </si>
+  <si>
+    <t>oos:finances/oos:budget/oos:code</t>
+  </si>
+  <si>
+    <t>oos:finances/oos:budget/oos:name</t>
   </si>
 </sst>
 </file>
@@ -579,11 +633,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,11 +645,12 @@
     <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.7109375" customWidth="1"/>
+    <col min="5" max="5" width="33.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -605,17 +660,20 @@
       <c r="C1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -625,17 +683,20 @@
       <c r="C2" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -645,17 +706,20 @@
       <c r="C3" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -665,17 +729,20 @@
       <c r="C4" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -685,17 +752,20 @@
       <c r="C5" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -705,17 +775,20 @@
       <c r="C6" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -723,273 +796,306 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" t="s">
-        <v>69</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding a few lines of config for notifications
</commit_message>
<xml_diff>
--- a/3-Unpack/how-I-parse-the-xml.xlsx
+++ b/3-Unpack/how-I-parse-the-xml.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="96">
   <si>
     <t>OutputTable</t>
   </si>
@@ -278,6 +278,30 @@
   </si>
   <si>
     <t>oos:finances/oos:budget/oos:name</t>
+  </si>
+  <si>
+    <t>notifications</t>
+  </si>
+  <si>
+    <t>notifications_&lt;region&gt;</t>
+  </si>
+  <si>
+    <t>/*/d1:notificationEF/oos:id</t>
+  </si>
+  <si>
+    <t>NotificationID</t>
+  </si>
+  <si>
+    <t>"13768"</t>
+  </si>
+  <si>
+    <t>/*/d1:notificationEF/oos:notificationNumber</t>
+  </si>
+  <si>
+    <t>oos:notificationNumber</t>
+  </si>
+  <si>
+    <t>NotificationNumber</t>
   </si>
 </sst>
 </file>
@@ -633,11 +657,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,37 +1088,83 @@
         <v>51</v>
       </c>
     </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>88</v>
+      </c>
       <c r="B20" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" t="s">
+        <v>94</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>43</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C22" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
         <v>57</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating parsing configuration to include more fields for notifications
</commit_message>
<xml_diff>
--- a/3-Unpack/how-I-parse-the-xml.xlsx
+++ b/3-Unpack/how-I-parse-the-xml.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="120">
   <si>
     <t>OutputTable</t>
   </si>
@@ -286,22 +286,94 @@
     <t>notifications_&lt;region&gt;</t>
   </si>
   <si>
-    <t>/*/d1:notificationEF/oos:id</t>
-  </si>
-  <si>
     <t>NotificationID</t>
   </si>
   <si>
     <t>"13768"</t>
   </si>
   <si>
-    <t>/*/d1:notificationEF/oos:notificationNumber</t>
-  </si>
-  <si>
     <t>oos:notificationNumber</t>
   </si>
   <si>
     <t>NotificationNumber</t>
+  </si>
+  <si>
+    <t>/*/d1:notificationXX/oos:id</t>
+  </si>
+  <si>
+    <t>/*/d1:notificationXX/oos:notificationNumber</t>
+  </si>
+  <si>
+    <t>/*/d1:notificationXX/oos:versionNumber</t>
+  </si>
+  <si>
+    <t>"1"</t>
+  </si>
+  <si>
+    <t>NotificationVersionNumber</t>
+  </si>
+  <si>
+    <t>"2011-01-21T15:31:06"</t>
+  </si>
+  <si>
+    <t>/*/d1:notificationXX/oos:placingWay/oos:name</t>
+  </si>
+  <si>
+    <t>oos:placingWay/oos:name</t>
+  </si>
+  <si>
+    <t>"Открытый конкурс"</t>
+  </si>
+  <si>
+    <t>NotificationPlacingWayName</t>
+  </si>
+  <si>
+    <t>/*/d1:notificationXX/oos:orderName</t>
+  </si>
+  <si>
+    <t>"Обязательное страхование авто гражданской ответственности владельцев транспортных средств"</t>
+  </si>
+  <si>
+    <t>oos:orderName</t>
+  </si>
+  <si>
+    <t>NotificationOrderName</t>
+  </si>
+  <si>
+    <t>/*/d1:notificationXX/oos:publishDate</t>
+  </si>
+  <si>
+    <t>NotificationPublishDate</t>
+  </si>
+  <si>
+    <t>notifications_lots_&lt;region&gt;</t>
+  </si>
+  <si>
+    <t>(Many lots to one notification)</t>
+  </si>
+  <si>
+    <t>/*/d1:notificationXX/oos:order/oos:placer/oos:regNum</t>
+  </si>
+  <si>
+    <t>oos:order/oos:placer/oos:regNum</t>
+  </si>
+  <si>
+    <t>"01761000012"</t>
+  </si>
+  <si>
+    <t>NotificationOrderPlacerRegNum</t>
+  </si>
+  <si>
+    <t>/*/d1:notificationXX/oos:order/oos:placer/oos:fullName</t>
+  </si>
+  <si>
+    <t>oos:order/oos:placer/oos:fullName</t>
+  </si>
+  <si>
+    <t>"Управление Федеральной налоговой службы по Республике Адыгея"</t>
+  </si>
+  <si>
+    <t>NotificationOrderPlacerFullName</t>
   </si>
 </sst>
 </file>
@@ -657,11 +729,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,19 +1168,19 @@
         <v>89</v>
       </c>
       <c r="C19" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D19" t="s">
         <v>71</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1119,10 +1191,10 @@
         <v>89</v>
       </c>
       <c r="C20" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>5</v>
@@ -1131,41 +1203,199 @@
         <v>7</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>88</v>
+      </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>108</v>
+      </c>
+      <c r="D22" t="s">
+        <v>73</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>46</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>88</v>
+      </c>
       <c r="B23" t="s">
-        <v>2</v>
+        <v>89</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
+        <v>100</v>
+      </c>
+      <c r="D23" t="s">
+        <v>101</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>15</v>
+        <v>102</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G23" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" t="s">
+        <v>112</v>
+      </c>
+      <c r="D25" t="s">
+        <v>113</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" t="s">
+        <v>116</v>
+      </c>
+      <c r="D26" t="s">
+        <v>117</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>57</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating one notification field in parsing config
</commit_message>
<xml_diff>
--- a/3-Unpack/how-I-parse-the-xml.xlsx
+++ b/3-Unpack/how-I-parse-the-xml.xlsx
@@ -298,9 +298,6 @@
     <t>NotificationNumber</t>
   </si>
   <si>
-    <t>/*/d1:notificationXX/oos:id</t>
-  </si>
-  <si>
     <t>/*/d1:notificationXX/oos:notificationNumber</t>
   </si>
   <si>
@@ -374,6 +371,9 @@
   </si>
   <si>
     <t>NotificationOrderPlacerFullName</t>
+  </si>
+  <si>
+    <t>//*/d1:notificationXX/oos:id</t>
   </si>
 </sst>
 </file>
@@ -733,7 +733,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,7 +1168,7 @@
         <v>89</v>
       </c>
       <c r="C19" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="D19" t="s">
         <v>71</v>
@@ -1191,7 +1191,7 @@
         <v>89</v>
       </c>
       <c r="C20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D20" t="s">
         <v>92</v>
@@ -1214,19 +1214,19 @@
         <v>89</v>
       </c>
       <c r="C21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D21" t="s">
         <v>75</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1237,19 +1237,19 @@
         <v>89</v>
       </c>
       <c r="C22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D22" t="s">
         <v>73</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1260,19 +1260,19 @@
         <v>89</v>
       </c>
       <c r="C23" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" t="s">
         <v>100</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1283,19 +1283,19 @@
         <v>89</v>
       </c>
       <c r="C24" t="s">
+        <v>103</v>
+      </c>
+      <c r="D24" t="s">
+        <v>105</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="D24" t="s">
-        <v>106</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1306,19 +1306,19 @@
         <v>89</v>
       </c>
       <c r="C25" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" t="s">
         <v>112</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1329,19 +1329,19 @@
         <v>89</v>
       </c>
       <c r="C26" t="s">
+        <v>115</v>
+      </c>
+      <c r="D26" t="s">
         <v>116</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1392,10 +1392,10 @@
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
+        <v>109</v>
+      </c>
+      <c r="C34" t="s">
         <v>110</v>
-      </c>
-      <c r="C34" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor change to first notification configuration field to parse
</commit_message>
<xml_diff>
--- a/3-Unpack/how-I-parse-the-xml.xlsx
+++ b/3-Unpack/how-I-parse-the-xml.xlsx
@@ -373,7 +373,7 @@
     <t>NotificationOrderPlacerFullName</t>
   </si>
   <si>
-    <t>//*/d1:notificationXX/oos:id</t>
+    <t>//*/d1:notificationZK/oos:id</t>
   </si>
 </sst>
 </file>
@@ -733,7 +733,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Running through another region and changing config XMLFieldPath
</commit_message>
<xml_diff>
--- a/3-Unpack/how-I-parse-the-xml.xlsx
+++ b/3-Unpack/how-I-parse-the-xml.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="121">
   <si>
     <t>OutputTable</t>
   </si>
@@ -298,12 +298,6 @@
     <t>NotificationNumber</t>
   </si>
   <si>
-    <t>/*/d1:notificationXX/oos:notificationNumber</t>
-  </si>
-  <si>
-    <t>/*/d1:notificationXX/oos:versionNumber</t>
-  </si>
-  <si>
     <t>"1"</t>
   </si>
   <si>
@@ -313,9 +307,6 @@
     <t>"2011-01-21T15:31:06"</t>
   </si>
   <si>
-    <t>/*/d1:notificationXX/oos:placingWay/oos:name</t>
-  </si>
-  <si>
     <t>oos:placingWay/oos:name</t>
   </si>
   <si>
@@ -325,9 +316,6 @@
     <t>NotificationPlacingWayName</t>
   </si>
   <si>
-    <t>/*/d1:notificationXX/oos:orderName</t>
-  </si>
-  <si>
     <t>"Обязательное страхование авто гражданской ответственности владельцев транспортных средств"</t>
   </si>
   <si>
@@ -337,9 +325,6 @@
     <t>NotificationOrderName</t>
   </si>
   <si>
-    <t>/*/d1:notificationXX/oos:publishDate</t>
-  </si>
-  <si>
     <t>NotificationPublishDate</t>
   </si>
   <si>
@@ -349,9 +334,6 @@
     <t>(Many lots to one notification)</t>
   </si>
   <si>
-    <t>/*/d1:notificationXX/oos:order/oos:placer/oos:regNum</t>
-  </si>
-  <si>
     <t>oos:order/oos:placer/oos:regNum</t>
   </si>
   <si>
@@ -361,9 +343,6 @@
     <t>NotificationOrderPlacerRegNum</t>
   </si>
   <si>
-    <t>/*/d1:notificationXX/oos:order/oos:placer/oos:fullName</t>
-  </si>
-  <si>
     <t>oos:order/oos:placer/oos:fullName</t>
   </si>
   <si>
@@ -374,6 +353,30 @@
   </si>
   <si>
     <t>//*/d1:notificationZK/oos:id</t>
+  </si>
+  <si>
+    <t>/*/*/oos:id</t>
+  </si>
+  <si>
+    <t>/*/*/oos:notificationNumber</t>
+  </si>
+  <si>
+    <t>/*/*/oos:versionNumber</t>
+  </si>
+  <si>
+    <t>/*/*/oos:publishDate</t>
+  </si>
+  <si>
+    <t>/*/*/oos:placingWay/oos:name</t>
+  </si>
+  <si>
+    <t>/*/*/oos:orderName</t>
+  </si>
+  <si>
+    <t>/*/*/oos:order/oos:placer/oos:regNum</t>
+  </si>
+  <si>
+    <t>/*/*/oos:order/oos:placer/oos:fullName</t>
   </si>
 </sst>
 </file>
@@ -733,7 +736,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,7 +1171,7 @@
         <v>89</v>
       </c>
       <c r="C19" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D19" t="s">
         <v>71</v>
@@ -1191,7 +1194,7 @@
         <v>89</v>
       </c>
       <c r="C20" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="D20" t="s">
         <v>92</v>
@@ -1214,19 +1217,19 @@
         <v>89</v>
       </c>
       <c r="C21" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="D21" t="s">
         <v>75</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1237,19 +1240,19 @@
         <v>89</v>
       </c>
       <c r="C22" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="D22" t="s">
         <v>73</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1260,19 +1263,19 @@
         <v>89</v>
       </c>
       <c r="C23" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="D23" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1283,19 +1286,19 @@
         <v>89</v>
       </c>
       <c r="C24" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="D24" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1306,19 +1309,19 @@
         <v>89</v>
       </c>
       <c r="C25" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="D25" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1329,19 +1332,19 @@
         <v>89</v>
       </c>
       <c r="C26" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="D26" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1349,6 +1352,9 @@
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>112</v>
+      </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
     </row>
@@ -1392,10 +1398,10 @@
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C34" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating config to pick up one product code
</commit_message>
<xml_diff>
--- a/3-Unpack/how-I-parse-the-xml.xlsx
+++ b/3-Unpack/how-I-parse-the-xml.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="125">
   <si>
     <t>OutputTable</t>
   </si>
@@ -377,6 +377,18 @@
   </si>
   <si>
     <t>/*/*/oos:order/oos:placer/oos:fullName</t>
+  </si>
+  <si>
+    <t>/*/*/oos:lots/oos:lot/oos:products/oos:product/oos:code</t>
+  </si>
+  <si>
+    <t>oos:lots/oos:lot/oos:products/oos:product/oos:code</t>
+  </si>
+  <si>
+    <t>"2320000"</t>
+  </si>
+  <si>
+    <t>NotificationMainLotMainProductCode</t>
   </si>
 </sst>
 </file>
@@ -732,11 +744,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1348,59 +1360,82 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
+      <c r="A27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D27" t="s">
+        <v>122</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>112</v>
-      </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>112</v>
+      </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" t="s">
-        <v>44</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>46</v>
-      </c>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="C32" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G32" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>57</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>104</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>105</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Starting work on the key-value version
</commit_message>
<xml_diff>
--- a/3-Unpack/how-I-parse-the-xml.xlsx
+++ b/3-Unpack/how-I-parse-the-xml.xlsx
@@ -747,8 +747,8 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updating parsing config with more fields and adding parsing diagnostic code
</commit_message>
<xml_diff>
--- a/3-Unpack/how-I-parse-the-xml.xlsx
+++ b/3-Unpack/how-I-parse-the-xml.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="238">
   <si>
     <t>OutputTable</t>
   </si>
@@ -388,7 +388,349 @@
     <t>"2320000"</t>
   </si>
   <si>
-    <t>NotificationMainLotMainProductCode</t>
+    <t>/*/d1:contract/oos:foundation/oos:order/oos:notificationNumber</t>
+  </si>
+  <si>
+    <t>oos:foundation/oos:order/oos:notificationNumber</t>
+  </si>
+  <si>
+    <t>"0376300000113000655"</t>
+  </si>
+  <si>
+    <t>ContractFoundationNotificationNumber</t>
+  </si>
+  <si>
+    <t>/*/*/oos:lots/oos:lot/oos:currency/oos:code</t>
+  </si>
+  <si>
+    <t>/*/*/oos:lots/oos:lot/oos:ordinalNumber</t>
+  </si>
+  <si>
+    <t>oos:lots/oos:lot/oos:ordinalNumber</t>
+  </si>
+  <si>
+    <t>NotificationLotProductCode</t>
+  </si>
+  <si>
+    <t>NotificationLotOrdinalNumber</t>
+  </si>
+  <si>
+    <t>/*/*/oos:lots/oos:lot/oos:subject</t>
+  </si>
+  <si>
+    <t>oos:lots/oos:lot/oos:subject</t>
+  </si>
+  <si>
+    <t>"запрос котировок на право заключения  государственного контракта на  поставку  нефтепродуктов с использованием топливных карт для нужд УФСБ России  по Республике Адыгея в I квартале 2011 года"</t>
+  </si>
+  <si>
+    <t>NotificationLotSubject</t>
+  </si>
+  <si>
+    <t>oos:lots/oos:lot/oos:currency/oos:code</t>
+  </si>
+  <si>
+    <t>NotificationLotCurrencyCode</t>
+  </si>
+  <si>
+    <t>/*/*/oos:lots/oos:lot/oos:products/oos:product/oos:name</t>
+  </si>
+  <si>
+    <t>oos:lots/oos:lot/oos:products/oos:product/oos:name</t>
+  </si>
+  <si>
+    <t>"Бензины автомобильные"</t>
+  </si>
+  <si>
+    <t>NotificationLotProductName</t>
+  </si>
+  <si>
+    <t>ManyPerDocument</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>"К запросу котировок не допускаются организации, сведения о которых содержатся в РНП"</t>
+  </si>
+  <si>
+    <t>NotificationLotNotificationPlacementFeatureName</t>
+  </si>
+  <si>
+    <t>/*/*/oos:lots/oos:lot/oos:customerRequirements/oos:customerRequirement/oos:quantity</t>
+  </si>
+  <si>
+    <t>oos:lots/oos:lot/oos:customerRequirements/oos:customerRequirement/oos:quantity</t>
+  </si>
+  <si>
+    <t>"Бензин «Премиум» ЕВРО – 95 или эквивалент - 5037 литров;
+Бензин  «Регуляр» ЕВРО- 92 или эквивалент - 5364 литров;
+Бензин «Нормаль» - 80  или эквивалент - 963 литров;
+Дизельное топливо ЕВРО или эквивалент - 50 литров."</t>
+  </si>
+  <si>
+    <t>NotificationLotCustomerRequirementQuantity</t>
+  </si>
+  <si>
+    <t>/*/*/oos:lots/oos:lot/oos:customerRequirements/oos:customerRequirement/oos:maxPrice</t>
+  </si>
+  <si>
+    <t>oos:lots/oos:lot/oos:customerRequirements/oos:customerRequirement/oos:maxPrice</t>
+  </si>
+  <si>
+    <t>"300000"</t>
+  </si>
+  <si>
+    <t>NotificationLotCustomerRequirementMaxPrice</t>
+  </si>
+  <si>
+    <t>/*/*/oos:lots/oos:lot/oos:customerRequirements/oos:customerRequirement/oos:customer/oos:regNum</t>
+  </si>
+  <si>
+    <t>oos:lots/oos:lot/oos:customerRequirements/oos:customerRequirement/oos:customer/oos:regNum</t>
+  </si>
+  <si>
+    <t>"01761000048"</t>
+  </si>
+  <si>
+    <t>NotificationLotCustomerRequirementCustomerRegNum</t>
+  </si>
+  <si>
+    <t>/*/*/oos:lots/oos:lot/oos:customerRequirements/oos:customerRequirement/oos:customer/oos:fullName</t>
+  </si>
+  <si>
+    <t>oos:lots/oos:lot/oos:customerRequirements/oos:customerRequirement/oos:customer/oos:fullName</t>
+  </si>
+  <si>
+    <t>"Управление Федеральной службы безопасности Российской Федерации по Республике Адыгея"</t>
+  </si>
+  <si>
+    <t>NotificationLotCustomerRequirementCustomerFullName</t>
+  </si>
+  <si>
+    <t>/*/*/oos:lots/oos:lot/oos:customerRequirements/oos:customerRequirement/oos:financeSource</t>
+  </si>
+  <si>
+    <t>oos:lots/oos:lot/oos:customerRequirements/oos:customerRequirement/oos:financeSource</t>
+  </si>
+  <si>
+    <t>NotificationLotCustomerRequirementFinanceSource</t>
+  </si>
+  <si>
+    <t>oos:foundation/oos:singleCustomer</t>
+  </si>
+  <si>
+    <t>ContractFoundationSingleCustomer</t>
+  </si>
+  <si>
+    <t>/*/d1:contract/oos:products/oos:product/oos:OKDP/oos:code</t>
+  </si>
+  <si>
+    <t>oos:products/oos:product/oos:OKDP/oos:code</t>
+  </si>
+  <si>
+    <t>"3010506"</t>
+  </si>
+  <si>
+    <t>ContractProductOKDPCode</t>
+  </si>
+  <si>
+    <t>/*/d1:contract/oos:products/oos:product/oos:OKEI/oos:code</t>
+  </si>
+  <si>
+    <t>oos:products/oos:product/oos:OKEI/oos:code</t>
+  </si>
+  <si>
+    <t>"796"</t>
+  </si>
+  <si>
+    <t>ContractProductOKEICode</t>
+  </si>
+  <si>
+    <t>/*/d1:contract/oos:products/oos:product/oos:OKDP/oos:name</t>
+  </si>
+  <si>
+    <t>oos:products/oos:product/oos:OKDP/oos:name</t>
+  </si>
+  <si>
+    <t>"Узлы и детали средств офсетной печати канцелярских"</t>
+  </si>
+  <si>
+    <t>ContractProductOKDPName</t>
+  </si>
+  <si>
+    <t>/*/d1:contract/oos:products/oos:product/oos:OKEI/oos:name</t>
+  </si>
+  <si>
+    <t>oos:products/oos:product/oos:OKEI/oos:name</t>
+  </si>
+  <si>
+    <t>"Штука"</t>
+  </si>
+  <si>
+    <t>ContractProductOKEIName</t>
+  </si>
+  <si>
+    <t>/*/d1:contract/oos:suppliers/oos:supplier/oos:participantType</t>
+  </si>
+  <si>
+    <t>oos:suppliers/oos:supplier/oos:participantType</t>
+  </si>
+  <si>
+    <t>"U"</t>
+  </si>
+  <si>
+    <t>ContractSupplierParticipantType</t>
+  </si>
+  <si>
+    <t>/*/d1:contract/oos:suppliers/oos:supplier/oos:inn</t>
+  </si>
+  <si>
+    <t>oos:suppliers/oos:supplier/oos:inn</t>
+  </si>
+  <si>
+    <t>"0105021223"</t>
+  </si>
+  <si>
+    <t>ContractSupplierParticipantINN</t>
+  </si>
+  <si>
+    <t>/*/d1:contract/oos:suppliers/oos:supplier/oos:kpp</t>
+  </si>
+  <si>
+    <t>oos:suppliers/oos:supplier/oos:kpp</t>
+  </si>
+  <si>
+    <t>ContractSupplierParticipantKPP</t>
+  </si>
+  <si>
+    <t>/*/d1:contract/oos:suppliers/oos:supplier/oos:organizationName</t>
+  </si>
+  <si>
+    <t>oos:suppliers/oos:supplier/oos:organizationName</t>
+  </si>
+  <si>
+    <t>"&amp;quot;Компьютер Хаус&amp;quot;"</t>
+  </si>
+  <si>
+    <t>ContractSupplierParticipantOrganizationName</t>
+  </si>
+  <si>
+    <t>/*/d1:contract/oos:finances/oos:budgetary/oos:KBK</t>
+  </si>
+  <si>
+    <t>oos:finances/oos:budgetary/oos:KBK</t>
+  </si>
+  <si>
+    <t>"15701130012700012223"</t>
+  </si>
+  <si>
+    <t>ContractFinanceBudgetaryKBK</t>
+  </si>
+  <si>
+    <t>/*/d1:contract/oos:finances/oos:budgetary/oos:price</t>
+  </si>
+  <si>
+    <t>oos:finances/oos:budgetary/oos:price</t>
+  </si>
+  <si>
+    <t>"85000"</t>
+  </si>
+  <si>
+    <t>ContractFinanceBudgetaryPrice</t>
+  </si>
+  <si>
+    <t>/*/d1:contract/oos:finances/oos:extrabudget/oos:name</t>
+  </si>
+  <si>
+    <t>oos:finances/oos:extrabudget/oos:name</t>
+  </si>
+  <si>
+    <t>"внебюджетные средства получателей средств федерального бюджета"</t>
+  </si>
+  <si>
+    <t>ContractFinanceExtraBudgetName</t>
+  </si>
+  <si>
+    <t>/*/d1:contract/oos:finances/oos:extrabudgetary/oos:KOSGU</t>
+  </si>
+  <si>
+    <t>oos:finances/oos:extrabudgetary/oos:KOSGU</t>
+  </si>
+  <si>
+    <t>"223"</t>
+  </si>
+  <si>
+    <t>ContractFinanceExtraBudgetaryKOSGU</t>
+  </si>
+  <si>
+    <t>/*/d1:contract/oos:finances/oos:extrabudgetary/oos:price</t>
+  </si>
+  <si>
+    <t>oos:finances/oos:extrabudgetary/oos:price</t>
+  </si>
+  <si>
+    <t>"155000"</t>
+  </si>
+  <si>
+    <t>ContractFinanceExtraBudgetaryPrice</t>
+  </si>
+  <si>
+    <t>/*/d1:contract/oos:products/oos:product/oos:price</t>
+  </si>
+  <si>
+    <t>oos:products/oos:product/oos:price</t>
+  </si>
+  <si>
+    <t>"4800"</t>
+  </si>
+  <si>
+    <t>ContractProductPrice</t>
+  </si>
+  <si>
+    <t>/*/d1:contract/oos:products/oos:product/oos:quantity</t>
+  </si>
+  <si>
+    <t>oos:products/oos:product/oos:quantity</t>
+  </si>
+  <si>
+    <t>"175"</t>
+  </si>
+  <si>
+    <t>ContractProductQuantity</t>
+  </si>
+  <si>
+    <t>/*/d1:contract/oos:products/oos:product/oos:sum</t>
+  </si>
+  <si>
+    <t>oos:products/oos:product/oos:sum</t>
+  </si>
+  <si>
+    <t>"840000"</t>
+  </si>
+  <si>
+    <t>ContractProductSum</t>
+  </si>
+  <si>
+    <t>/*/d1:contract/oos:currentContractStage</t>
+  </si>
+  <si>
+    <t>oos:currentContractStage</t>
+  </si>
+  <si>
+    <t>"E"</t>
+  </si>
+  <si>
+    <t>ContractCurrentContractStage</t>
+  </si>
+  <si>
+    <t>/*/*/oos:lots/oos:lot/oos:notificationFeatures/oos:notificationFeature/oos:placementFeature/oos:name</t>
+  </si>
+  <si>
+    <t>oos:lots/oos:lot/oos:notificationFeatures/oos:notificationFeature/oos:placementFeature/oos:name</t>
   </si>
 </sst>
 </file>
@@ -432,7 +774,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -440,6 +782,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -744,11 +1089,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,7 +1106,7 @@
     <col min="7" max="7" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -783,8 +1128,11 @@
       <c r="G1" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -806,8 +1154,11 @@
       <c r="G2" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -829,8 +1180,11 @@
       <c r="G3" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -852,8 +1206,11 @@
       <c r="G4" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -875,8 +1232,11 @@
       <c r="G5" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -898,8 +1258,11 @@
       <c r="G6" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -907,22 +1270,25 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>124</v>
       </c>
       <c r="D7" t="s">
-        <v>77</v>
+        <v>125</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>25</v>
+        <v>126</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -930,22 +1296,25 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>78</v>
+        <v>167</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -953,22 +1322,25 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -976,91 +1348,103 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="H12" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
         <v>62</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D13" t="s">
         <v>81</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" t="s">
-        <v>76</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" t="s">
-        <v>82</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1068,374 +1452,1170 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D14" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="H16" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
         <v>66</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D17" t="s">
         <v>84</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="H17" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
         <v>67</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D18" t="s">
         <v>85</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" t="s">
-        <v>86</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" t="s">
-        <v>69</v>
-      </c>
-      <c r="D18" t="s">
-        <v>87</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>88</v>
-      </c>
-      <c r="B19" t="s">
-        <v>89</v>
-      </c>
-      <c r="C19" t="s">
-        <v>113</v>
-      </c>
-      <c r="D19" t="s">
-        <v>71</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C20" t="s">
-        <v>114</v>
-      </c>
-      <c r="D20" t="s">
-        <v>92</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" s="1" t="s">
+      <c r="H20" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>200</v>
+      </c>
+      <c r="D21" t="s">
+        <v>201</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>88</v>
-      </c>
-      <c r="B21" t="s">
-        <v>89</v>
-      </c>
-      <c r="C21" t="s">
-        <v>115</v>
-      </c>
-      <c r="D21" t="s">
-        <v>75</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="G21" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>89</v>
+        <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>116</v>
+        <v>204</v>
       </c>
       <c r="D22" t="s">
-        <v>73</v>
+        <v>205</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>96</v>
+        <v>206</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>117</v>
+        <v>208</v>
       </c>
       <c r="D23" t="s">
-        <v>97</v>
+        <v>209</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>98</v>
+        <v>210</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>118</v>
+        <v>212</v>
       </c>
       <c r="D24" t="s">
-        <v>101</v>
+        <v>213</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>100</v>
+        <v>214</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>89</v>
+        <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>119</v>
+        <v>216</v>
       </c>
       <c r="D25" t="s">
-        <v>106</v>
+        <v>217</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>107</v>
+        <v>218</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>120</v>
+        <v>169</v>
       </c>
       <c r="D26" t="s">
-        <v>109</v>
+        <v>170</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>110</v>
+        <v>171</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>89</v>
+        <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>121</v>
+        <v>177</v>
       </c>
       <c r="D27" t="s">
-        <v>122</v>
+        <v>178</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>123</v>
+        <v>179</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>173</v>
+      </c>
+      <c r="D28" t="s">
+        <v>174</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>2</v>
+      </c>
       <c r="C29" t="s">
-        <v>112</v>
-      </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+      <c r="D29" t="s">
+        <v>182</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>220</v>
+      </c>
+      <c r="D30" t="s">
+        <v>221</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>224</v>
+      </c>
+      <c r="D31" t="s">
+        <v>225</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>44</v>
+        <v>228</v>
+      </c>
+      <c r="D32" t="s">
+        <v>229</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>45</v>
+        <v>230</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>1</v>
+      </c>
       <c r="B33" t="s">
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>57</v>
+        <v>185</v>
+      </c>
+      <c r="D33" t="s">
+        <v>186</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>15</v>
+        <v>187</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G33" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>189</v>
+      </c>
+      <c r="D34" t="s">
+        <v>190</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>193</v>
+      </c>
+      <c r="D35" t="s">
+        <v>194</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>196</v>
+      </c>
+      <c r="D36" t="s">
+        <v>197</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>232</v>
+      </c>
+      <c r="D37" t="s">
+        <v>233</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" t="s">
+        <v>71</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" t="s">
+        <v>92</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>88</v>
+      </c>
+      <c r="B40" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" t="s">
+        <v>115</v>
+      </c>
+      <c r="D40" t="s">
+        <v>75</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C41" t="s">
+        <v>116</v>
+      </c>
+      <c r="D41" t="s">
+        <v>73</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>88</v>
+      </c>
+      <c r="B42" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" t="s">
+        <v>117</v>
+      </c>
+      <c r="D42" t="s">
+        <v>97</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>88</v>
+      </c>
+      <c r="B43" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" t="s">
+        <v>118</v>
+      </c>
+      <c r="D43" t="s">
+        <v>101</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>88</v>
+      </c>
+      <c r="B44" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" t="s">
+        <v>119</v>
+      </c>
+      <c r="D44" t="s">
+        <v>106</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" t="s">
+        <v>120</v>
+      </c>
+      <c r="D45" t="s">
+        <v>109</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" t="s">
+        <v>129</v>
+      </c>
+      <c r="D46" t="s">
+        <v>130</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" t="s">
+        <v>133</v>
+      </c>
+      <c r="D47" t="s">
+        <v>134</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" t="s">
+        <v>128</v>
+      </c>
+      <c r="D48" t="s">
+        <v>137</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>88</v>
+      </c>
+      <c r="B49" t="s">
+        <v>89</v>
+      </c>
+      <c r="C49" t="s">
+        <v>121</v>
+      </c>
+      <c r="D49" t="s">
+        <v>122</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" t="s">
+        <v>89</v>
+      </c>
+      <c r="C50" t="s">
+        <v>139</v>
+      </c>
+      <c r="D50" t="s">
+        <v>140</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" t="s">
+        <v>89</v>
+      </c>
+      <c r="C51" t="s">
+        <v>236</v>
+      </c>
+      <c r="D51" t="s">
+        <v>237</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>88</v>
+      </c>
+      <c r="B52" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52" t="s">
+        <v>148</v>
+      </c>
+      <c r="D52" t="s">
+        <v>149</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" t="s">
+        <v>89</v>
+      </c>
+      <c r="C53" t="s">
+        <v>152</v>
+      </c>
+      <c r="D53" t="s">
+        <v>153</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>88</v>
+      </c>
+      <c r="B54" t="s">
+        <v>89</v>
+      </c>
+      <c r="C54" t="s">
+        <v>156</v>
+      </c>
+      <c r="D54" t="s">
+        <v>157</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>88</v>
+      </c>
+      <c r="B55" t="s">
+        <v>89</v>
+      </c>
+      <c r="C55" t="s">
+        <v>160</v>
+      </c>
+      <c r="D55" t="s">
+        <v>161</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>88</v>
+      </c>
+      <c r="B56" t="s">
+        <v>89</v>
+      </c>
+      <c r="C56" t="s">
+        <v>164</v>
+      </c>
+      <c r="D56" t="s">
+        <v>165</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>112</v>
+      </c>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>43</v>
+      </c>
+      <c r="C61" t="s">
+        <v>44</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" t="s">
+        <v>57</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G62" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
         <v>104</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C64" t="s">
         <v>105</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding notification URL on zakupki.gov to parser config
</commit_message>
<xml_diff>
--- a/3-Unpack/how-I-parse-the-xml.xlsx
+++ b/3-Unpack/how-I-parse-the-xml.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26519"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="100" windowWidth="14800" windowHeight="8020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="242">
   <si>
     <t>OutputTable</t>
   </si>
@@ -731,13 +736,25 @@
   </si>
   <si>
     <t>oos:lots/oos:lot/oos:notificationFeatures/oos:notificationFeature/oos:placementFeature/oos:name</t>
+  </si>
+  <si>
+    <t>/*/*/oos:href</t>
+  </si>
+  <si>
+    <t>oos:href</t>
+  </si>
+  <si>
+    <t>"http://zakupki.gov.ru/pgz/public/action/orders/info/common_info/show?notificationId=27923"</t>
+  </si>
+  <si>
+    <t>NotificationPage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -749,6 +766,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -771,8 +804,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -786,7 +821,9 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -845,7 +882,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -880,7 +917,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1089,24 +1126,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.7109375" customWidth="1"/>
-    <col min="5" max="5" width="33.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.6640625" customWidth="1"/>
+    <col min="5" max="5" width="33.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1132,7 +1169,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1158,7 +1195,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1184,7 +1221,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1210,7 +1247,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1236,7 +1273,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1262,7 +1299,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1288,7 +1325,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1314,7 +1351,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1340,7 +1377,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1366,7 +1403,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1392,7 +1429,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1418,7 +1455,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -1444,7 +1481,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1470,7 +1507,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -1496,7 +1533,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -1522,7 +1559,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -1548,7 +1585,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -1574,7 +1611,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -1600,7 +1637,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -1626,7 +1663,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -1652,7 +1689,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -1678,7 +1715,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -1704,7 +1741,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -1730,7 +1767,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -1756,7 +1793,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -1782,7 +1819,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -1808,7 +1845,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -1834,7 +1871,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -1860,7 +1897,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -1886,7 +1923,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -1912,7 +1949,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -1938,7 +1975,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -1964,7 +2001,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -1990,7 +2027,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -2016,7 +2053,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -2042,7 +2079,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -2068,7 +2105,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>88</v>
       </c>
@@ -2094,7 +2131,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>88</v>
       </c>
@@ -2120,7 +2157,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>88</v>
       </c>
@@ -2146,7 +2183,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>88</v>
       </c>
@@ -2172,7 +2209,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>88</v>
       </c>
@@ -2198,7 +2235,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
         <v>88</v>
       </c>
@@ -2224,7 +2261,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
         <v>88</v>
       </c>
@@ -2250,7 +2287,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
         <v>88</v>
       </c>
@@ -2276,7 +2313,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
         <v>88</v>
       </c>
@@ -2284,25 +2321,25 @@
         <v>89</v>
       </c>
       <c r="C46" t="s">
-        <v>129</v>
+        <v>238</v>
       </c>
       <c r="D46" t="s">
-        <v>130</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>94</v>
+        <v>239</v>
+      </c>
+      <c r="E46" t="s">
+        <v>240</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>132</v>
+        <v>241</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
         <v>88</v>
       </c>
@@ -2310,25 +2347,25 @@
         <v>89</v>
       </c>
       <c r="C47" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D47" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>135</v>
+        <v>94</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
         <v>88</v>
       </c>
@@ -2336,25 +2373,25 @@
         <v>89</v>
       </c>
       <c r="C48" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="D48" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>37</v>
+        <v>135</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
         <v>88</v>
       </c>
@@ -2362,25 +2399,25 @@
         <v>89</v>
       </c>
       <c r="C49" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="D49" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>123</v>
+        <v>37</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>88</v>
       </c>
@@ -2388,25 +2425,25 @@
         <v>89</v>
       </c>
       <c r="C50" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="D50" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
         <v>88</v>
       </c>
@@ -2414,25 +2451,25 @@
         <v>89</v>
       </c>
       <c r="C51" t="s">
-        <v>236</v>
+        <v>139</v>
       </c>
       <c r="D51" t="s">
-        <v>237</v>
+        <v>140</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
         <v>88</v>
       </c>
@@ -2440,25 +2477,25 @@
         <v>89</v>
       </c>
       <c r="C52" t="s">
-        <v>148</v>
+        <v>236</v>
       </c>
       <c r="D52" t="s">
-        <v>149</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>150</v>
+        <v>237</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>146</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="112">
       <c r="A53" t="s">
         <v>88</v>
       </c>
@@ -2466,25 +2503,25 @@
         <v>89</v>
       </c>
       <c r="C53" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D53" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
         <v>88</v>
       </c>
@@ -2492,25 +2529,25 @@
         <v>89</v>
       </c>
       <c r="C54" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D54" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="A55" t="s">
         <v>88</v>
       </c>
@@ -2518,25 +2555,25 @@
         <v>89</v>
       </c>
       <c r="C55" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D55" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="42">
       <c r="A56" t="s">
         <v>88</v>
       </c>
@@ -2544,83 +2581,114 @@
         <v>89</v>
       </c>
       <c r="C56" t="s">
+        <v>160</v>
+      </c>
+      <c r="D56" t="s">
+        <v>161</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" t="s">
+        <v>88</v>
+      </c>
+      <c r="B57" t="s">
+        <v>89</v>
+      </c>
+      <c r="C57" t="s">
         <v>164</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D57" t="s">
         <v>165</v>
       </c>
-      <c r="E56" s="5" t="s">
+      <c r="E57" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="F57" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G56" s="1" t="s">
+      <c r="G57" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="H56" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C58" t="s">
-        <v>112</v>
-      </c>
+      <c r="H57" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8">
+      <c r="C59" t="s">
+        <v>112</v>
+      </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
+    <row r="60" spans="1:8">
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="B62" t="s">
         <v>43</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C62" t="s">
         <v>44</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="E62" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>2</v>
-      </c>
-      <c r="C62" t="s">
-        <v>57</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G62" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="B63" t="s">
+        <v>2</v>
+      </c>
+      <c r="C63" t="s">
+        <v>57</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G63" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
+    <row r="65" spans="2:3">
+      <c r="B65" t="s">
         <v>104</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C65" t="s">
         <v>105</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Altering order of parser config and adding commentary to data quality step
</commit_message>
<xml_diff>
--- a/3-Unpack/how-I-parse-the-xml.xlsx
+++ b/3-Unpack/how-I-parse-the-xml.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26519"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="100" windowWidth="14800" windowHeight="8020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,43 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="C4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+versionNumber needs to be third in list for parser to work. Order should be:
+1) oos:id
+2) business key (eg oos:regNum)
+3) oos:versionNumber</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="242">
   <si>
@@ -754,7 +791,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -786,6 +823,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -804,8 +854,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -821,9 +873,11 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1125,12 +1179,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G46" sqref="G46"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1229,19 +1283,19 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>11</v>
+        <v>75</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>144</v>
@@ -1255,19 +1309,19 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>13</v>
+        <v>73</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>144</v>
@@ -1281,19 +1335,19 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>144</v>
@@ -2685,6 +2739,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Further work hardening the parser for the output I need
</commit_message>
<xml_diff>
--- a/3-Unpack/how-I-parse-the-xml.xlsx
+++ b/3-Unpack/how-I-parse-the-xml.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26519"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26929"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15860"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="246">
   <si>
     <t>OutputTable</t>
   </si>
@@ -323,9 +323,6 @@
   </si>
   <si>
     <t>notifications</t>
-  </si>
-  <si>
-    <t>notifications_&lt;region&gt;</t>
   </si>
   <si>
     <t>NotificationID</t>
@@ -785,13 +782,28 @@
   </si>
   <si>
     <t>NotificationPage</t>
+  </si>
+  <si>
+    <t>VariableNameShort</t>
+  </si>
+  <si>
+    <t>NotificationLotMaxPrice</t>
+  </si>
+  <si>
+    <t>notification_lots</t>
+  </si>
+  <si>
+    <t>notification_lot_products</t>
+  </si>
+  <si>
+    <t>notification_requirements</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -836,6 +848,21 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -854,14 +881,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -872,12 +919,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1180,24 +1249,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H65"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.5" customWidth="1"/>
     <col min="4" max="4" width="47.6640625" customWidth="1"/>
     <col min="5" max="5" width="33.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1">
+    <row r="1" spans="1:9" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1219,11 +1289,14 @@
       <c r="G1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="H1" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1245,11 +1318,14 @@
       <c r="G2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="H2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1271,11 +1347,14 @@
       <c r="G3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="H3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1297,11 +1376,14 @@
       <c r="G4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="H4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1323,11 +1405,14 @@
       <c r="G5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="H5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1349,11 +1434,14 @@
       <c r="G6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="H6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1361,25 +1449,28 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" t="s">
         <v>124</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>126</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1390,7 +1481,7 @@
         <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>15</v>
@@ -1399,13 +1490,16 @@
         <v>16</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>167</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1427,11 +1521,14 @@
       <c r="G9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="H9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1453,11 +1550,14 @@
       <c r="G10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="H10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1479,11 +1579,14 @@
       <c r="G11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="H11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1505,11 +1608,14 @@
       <c r="G12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="H12" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -1531,11 +1637,14 @@
       <c r="G13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="H13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1557,11 +1666,14 @@
       <c r="G14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="H14" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -1583,11 +1695,14 @@
       <c r="G15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="H15" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -1609,11 +1724,14 @@
       <c r="G16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="H16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -1635,11 +1753,14 @@
       <c r="G17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="H17" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -1661,11 +1782,14 @@
       <c r="G18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="H18" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -1687,11 +1811,14 @@
       <c r="G19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="H19" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -1713,11 +1840,14 @@
       <c r="G20" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="H20" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -1725,129 +1855,144 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
+        <v>199</v>
+      </c>
+      <c r="D21" t="s">
         <v>200</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G21" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
         <v>203</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>204</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>206</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G22" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
         <v>207</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
-        <v>2</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>208</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>210</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G23" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
         <v>211</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>212</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>214</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G24" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
         <v>215</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" t="s">
-        <v>2</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>216</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>218</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -1855,25 +2000,28 @@
         <v>2</v>
       </c>
       <c r="C26" t="s">
+        <v>168</v>
+      </c>
+      <c r="D26" t="s">
         <v>169</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+        <v>171</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -1881,25 +2029,28 @@
         <v>2</v>
       </c>
       <c r="C27" t="s">
+        <v>176</v>
+      </c>
+      <c r="D27" t="s">
         <v>177</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>179</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -1907,25 +2058,28 @@
         <v>2</v>
       </c>
       <c r="C28" t="s">
+        <v>172</v>
+      </c>
+      <c r="D28" t="s">
         <v>173</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>175</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -1933,25 +2087,28 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
+        <v>180</v>
+      </c>
+      <c r="D29" t="s">
         <v>181</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>183</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -1959,77 +2116,86 @@
         <v>2</v>
       </c>
       <c r="C30" t="s">
+        <v>219</v>
+      </c>
+      <c r="D30" t="s">
         <v>220</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G30" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
         <v>223</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" t="s">
-        <v>1</v>
-      </c>
-      <c r="B31" t="s">
-        <v>2</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>224</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G31" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
         <v>227</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32" t="s">
-        <v>2</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>228</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <v>230</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -2037,62 +2203,68 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
+        <v>184</v>
+      </c>
+      <c r="D33" t="s">
         <v>185</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G33" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
         <v>188</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B34" t="s">
-        <v>2</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>189</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G34" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
         <v>192</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" t="s">
-        <v>1</v>
-      </c>
-      <c r="B35" t="s">
-        <v>2</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>193</v>
-      </c>
-      <c r="D35" t="s">
-        <v>194</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>31</v>
@@ -2101,39 +2273,45 @@
         <v>16</v>
       </c>
       <c r="G35" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
         <v>195</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" t="s">
-        <v>1</v>
-      </c>
-      <c r="B36" t="s">
-        <v>2</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>196</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>198</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+        <v>198</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -2141,62 +2319,68 @@
         <v>2</v>
       </c>
       <c r="C37" t="s">
+        <v>231</v>
+      </c>
+      <c r="D37" t="s">
         <v>232</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>234</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+        <v>234</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
         <v>88</v>
       </c>
       <c r="B38" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D38" t="s">
         <v>71</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+        <v>89</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
         <v>88</v>
       </c>
       <c r="B39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C39" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D39" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>5</v>
@@ -2205,258 +2389,288 @@
         <v>7</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+        <v>92</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" t="s">
         <v>88</v>
       </c>
       <c r="B40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C40" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D40" t="s">
         <v>75</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
+        <v>94</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
         <v>88</v>
       </c>
       <c r="B41" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C41" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D41" t="s">
         <v>73</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+        <v>102</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
         <v>88</v>
       </c>
       <c r="B42" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D42" t="s">
+        <v>96</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+        <v>98</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
         <v>88</v>
       </c>
       <c r="B43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C43" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+        <v>101</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
         <v>88</v>
       </c>
       <c r="B44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D44" t="s">
+        <v>105</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+        <v>107</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
         <v>88</v>
       </c>
       <c r="B45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C45" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D45" t="s">
+        <v>108</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+        <v>110</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" t="s">
         <v>88</v>
       </c>
       <c r="B46" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C46" t="s">
+        <v>237</v>
+      </c>
+      <c r="D46" t="s">
         <v>238</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>239</v>
-      </c>
-      <c r="E46" t="s">
-        <v>240</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
+        <v>240</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47" t="s">
         <v>88</v>
       </c>
       <c r="B47" t="s">
-        <v>89</v>
+        <v>243</v>
       </c>
       <c r="C47" t="s">
+        <v>128</v>
+      </c>
+      <c r="D47" t="s">
         <v>129</v>
       </c>
-      <c r="D47" t="s">
-        <v>130</v>
-      </c>
       <c r="E47" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
+        <v>131</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48" t="s">
         <v>88</v>
       </c>
       <c r="B48" t="s">
-        <v>89</v>
+        <v>243</v>
       </c>
       <c r="C48" t="s">
+        <v>132</v>
+      </c>
+      <c r="D48" t="s">
         <v>133</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
+        <v>135</v>
+      </c>
+      <c r="H48" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
         <v>88</v>
       </c>
       <c r="B49" t="s">
-        <v>89</v>
+        <v>243</v>
       </c>
       <c r="C49" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D49" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>37</v>
@@ -2465,206 +2679,230 @@
         <v>16</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
+        <v>137</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50" t="s">
         <v>88</v>
       </c>
       <c r="B50" t="s">
-        <v>89</v>
+        <v>244</v>
       </c>
       <c r="C50" t="s">
+        <v>120</v>
+      </c>
+      <c r="D50" t="s">
         <v>121</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
+        <v>130</v>
+      </c>
+      <c r="H50" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51" t="s">
         <v>88</v>
       </c>
       <c r="B51" t="s">
-        <v>89</v>
+        <v>244</v>
       </c>
       <c r="C51" t="s">
+        <v>138</v>
+      </c>
+      <c r="D51" t="s">
         <v>139</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
+        <v>141</v>
+      </c>
+      <c r="H51" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52" t="s">
         <v>88</v>
       </c>
       <c r="B52" t="s">
-        <v>89</v>
+        <v>243</v>
       </c>
       <c r="C52" t="s">
+        <v>235</v>
+      </c>
+      <c r="D52" t="s">
         <v>236</v>
       </c>
-      <c r="D52" t="s">
-        <v>237</v>
-      </c>
       <c r="E52" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="112">
+        <v>146</v>
+      </c>
+      <c r="H52" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="112">
       <c r="A53" t="s">
         <v>88</v>
       </c>
       <c r="B53" t="s">
-        <v>89</v>
+        <v>245</v>
       </c>
       <c r="C53" t="s">
+        <v>147</v>
+      </c>
+      <c r="D53" t="s">
         <v>148</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" s="5" t="s">
         <v>149</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>150</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
+        <v>150</v>
+      </c>
+      <c r="H53" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
       <c r="A54" t="s">
         <v>88</v>
       </c>
       <c r="B54" t="s">
-        <v>89</v>
+        <v>245</v>
       </c>
       <c r="C54" t="s">
+        <v>151</v>
+      </c>
+      <c r="D54" t="s">
         <v>152</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" s="5" t="s">
         <v>153</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>154</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8">
+        <v>154</v>
+      </c>
+      <c r="H54" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
       <c r="A55" t="s">
         <v>88</v>
       </c>
       <c r="B55" t="s">
-        <v>89</v>
+        <v>245</v>
       </c>
       <c r="C55" t="s">
+        <v>155</v>
+      </c>
+      <c r="D55" t="s">
         <v>156</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" s="5" t="s">
         <v>157</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>158</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="42">
+        <v>158</v>
+      </c>
+      <c r="H55" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="42">
       <c r="A56" t="s">
         <v>88</v>
       </c>
       <c r="B56" t="s">
-        <v>89</v>
+        <v>245</v>
       </c>
       <c r="C56" t="s">
+        <v>159</v>
+      </c>
+      <c r="D56" t="s">
         <v>160</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" s="5" t="s">
         <v>161</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>162</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
+        <v>162</v>
+      </c>
+      <c r="H56" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57" t="s">
         <v>88</v>
       </c>
       <c r="B57" t="s">
-        <v>89</v>
+        <v>245</v>
       </c>
       <c r="C57" t="s">
+        <v>163</v>
+      </c>
+      <c r="D57" t="s">
         <v>164</v>
-      </c>
-      <c r="D57" t="s">
-        <v>165</v>
       </c>
       <c r="E57" s="5" t="s">
         <v>50</v>
@@ -2673,28 +2911,37 @@
         <v>16</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8">
+        <v>165</v>
+      </c>
+      <c r="H57" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
-    </row>
-    <row r="59" spans="1:8">
+      <c r="H58" s="7"/>
+    </row>
+    <row r="59" spans="1:9">
       <c r="C59" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
-    </row>
-    <row r="60" spans="1:8">
+      <c r="H59" s="7"/>
+    </row>
+    <row r="60" spans="1:9">
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
-    </row>
-    <row r="62" spans="1:8">
+      <c r="H60" s="7"/>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="H61" s="7"/>
+    </row>
+    <row r="62" spans="1:9">
       <c r="B62" t="s">
         <v>43</v>
       </c>
@@ -2710,8 +2957,11 @@
       <c r="G62" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="63" spans="1:8">
+      <c r="H62" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
       <c r="B63" t="s">
         <v>2</v>
       </c>
@@ -2727,14 +2977,21 @@
       <c r="G63" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="65" spans="2:3">
+      <c r="H63" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="H64" s="7"/>
+    </row>
+    <row r="65" spans="2:8">
       <c r="B65" t="s">
+        <v>103</v>
+      </c>
+      <c r="C65" t="s">
         <v>104</v>
       </c>
-      <c r="C65" t="s">
-        <v>105</v>
-      </c>
+      <c r="H65" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Correcting parsing config and setup scripts
</commit_message>
<xml_diff>
--- a/3-Unpack/how-I-parse-the-xml.xlsx
+++ b/3-Unpack/how-I-parse-the-xml.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27309"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/shaun/git/shaun-mcgirr-dissertation/3-Unpack/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15860"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -1252,11 +1260,11 @@
   <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B53" sqref="B53"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
@@ -1267,7 +1275,7 @@
     <col min="8" max="8" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1296,7 +1304,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1325,7 +1333,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1354,7 +1362,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1383,7 +1391,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1412,7 +1420,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1441,7 +1449,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1470,7 +1478,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1499,7 +1507,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1528,7 +1536,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1557,7 +1565,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1586,7 +1594,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1615,7 +1623,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -1644,7 +1652,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1673,7 +1681,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -1702,7 +1710,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -1731,7 +1739,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -1760,7 +1768,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -1789,7 +1797,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -1818,7 +1826,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -1847,7 +1855,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -1876,7 +1884,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -1905,7 +1913,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -1934,7 +1942,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -1963,7 +1971,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -1992,7 +2000,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -2021,7 +2029,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -2050,7 +2058,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -2079,7 +2087,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -2108,7 +2116,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -2137,7 +2145,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -2166,7 +2174,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -2195,7 +2203,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -2224,7 +2232,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -2253,7 +2261,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -2282,7 +2290,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -2311,7 +2319,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -2337,10 +2345,10 @@
         <v>234</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>88</v>
       </c>
@@ -2369,7 +2377,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>88</v>
       </c>
@@ -2398,7 +2406,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>88</v>
       </c>
@@ -2427,7 +2435,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>88</v>
       </c>
@@ -2456,7 +2464,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>88</v>
       </c>
@@ -2485,7 +2493,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>88</v>
       </c>
@@ -2514,7 +2522,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>88</v>
       </c>
@@ -2543,7 +2551,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>88</v>
       </c>
@@ -2572,7 +2580,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>88</v>
       </c>
@@ -2601,7 +2609,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>88</v>
       </c>
@@ -2630,7 +2638,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>88</v>
       </c>
@@ -2659,7 +2667,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>88</v>
       </c>
@@ -2688,7 +2696,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>88</v>
       </c>
@@ -2717,7 +2725,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>88</v>
       </c>
@@ -2746,7 +2754,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>88</v>
       </c>
@@ -2775,7 +2783,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="112">
+    <row r="53" spans="1:9" ht="120" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>88</v>
       </c>
@@ -2804,7 +2812,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>88</v>
       </c>
@@ -2833,7 +2841,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>88</v>
       </c>
@@ -2862,7 +2870,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="42">
+    <row r="56" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>88</v>
       </c>
@@ -2891,7 +2899,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>88</v>
       </c>
@@ -2920,12 +2928,12 @@
         <v>144</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="7"/>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C59" t="s">
         <v>111</v>
       </c>
@@ -2933,15 +2941,15 @@
       <c r="G59" s="1"/>
       <c r="H59" s="7"/>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
       <c r="H60" s="7"/>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H61" s="7"/>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>43</v>
       </c>
@@ -2961,7 +2969,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>2</v>
       </c>
@@ -2981,10 +2989,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H64" s="7"/>
     </row>
-    <row r="65" spans="2:8">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>103</v>
       </c>
@@ -2997,10 +3005,5 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding singleCustomerReason to contracts parser
</commit_message>
<xml_diff>
--- a/3-Unpack/how-I-parse-the-xml.xlsx
+++ b/3-Unpack/how-I-parse-the-xml.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15860"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="294">
   <si>
     <t>OutputTable</t>
   </si>
@@ -805,6 +805,150 @@
   </si>
   <si>
     <t>notification_requirements</t>
+  </si>
+  <si>
+    <t>protocols</t>
+  </si>
+  <si>
+    <t>protocols_&lt;region&gt;</t>
+  </si>
+  <si>
+    <t>/*/*/oos:protocolNumber</t>
+  </si>
+  <si>
+    <t>/*/*/oos:foundationProtocolNumber</t>
+  </si>
+  <si>
+    <t>oos:protocolNumber</t>
+  </si>
+  <si>
+    <t>oos:foundationProtocolNumber</t>
+  </si>
+  <si>
+    <t>"0373100045312000060"</t>
+  </si>
+  <si>
+    <t>"0373100045312000060-2"</t>
+  </si>
+  <si>
+    <t>"0373100045312000060-1"</t>
+  </si>
+  <si>
+    <t>ProtocolNotificationNumber</t>
+  </si>
+  <si>
+    <t>ProtocolProtocolNumber</t>
+  </si>
+  <si>
+    <t>ProtocolFoundationProtocolNumber</t>
+  </si>
+  <si>
+    <t>ProtocolVersionNumber</t>
+  </si>
+  <si>
+    <t>/*/*/oos:protocolDate</t>
+  </si>
+  <si>
+    <t>oos:protocolDate</t>
+  </si>
+  <si>
+    <t>"2012-04-24T15:44:15Z"</t>
+  </si>
+  <si>
+    <t>ProtocolDate</t>
+  </si>
+  <si>
+    <t>/*/*/oos:signDate</t>
+  </si>
+  <si>
+    <t>ProtocolSignDate</t>
+  </si>
+  <si>
+    <t>ProtocolPublishDate</t>
+  </si>
+  <si>
+    <t>http://zakupki.gov.ru/pgz/public/action/orders/info/common_info/show?notificationId=3051805</t>
+  </si>
+  <si>
+    <t>ProtocolPage</t>
+  </si>
+  <si>
+    <t>/*/*/oos:protocolLots/oos:protocolLot/oos:lotNumber</t>
+  </si>
+  <si>
+    <t>oos:protocolLots/oos:protocolLot/oos:lotNumber</t>
+  </si>
+  <si>
+    <t>ProtocolLotNumber</t>
+  </si>
+  <si>
+    <t>/*/*/oos:protocolLots/oos:protocolLot/oos:applications/oos:application/oos:journalNumber</t>
+  </si>
+  <si>
+    <t>/*/*/oos:protocolLots/oos:protocolLot/oos:applications/oos:application/oos:admitted</t>
+  </si>
+  <si>
+    <t>/*/*/oos:protocolLots/oos:protocolLot/oos:applications/oos:application/oos:appRating</t>
+  </si>
+  <si>
+    <t>oos:protocolLots/oos:protocolLot/oos:applications/oos:application/oos:journalNumber</t>
+  </si>
+  <si>
+    <t>oos:protocolLots/oos:protocolLot/oos:applications/oos:application/oos:admitted</t>
+  </si>
+  <si>
+    <t>oos:protocolLots/oos:protocolLot/oos:applications/oos:application/oos:appRating</t>
+  </si>
+  <si>
+    <t>/*/*/oos:protocolLots/oos:protocolLot/oos:applications/oos:application/oos:applicationParticipants/oos:applicationParticipant/oos:inn</t>
+  </si>
+  <si>
+    <t>/*/*/oos:protocolLots/oos:protocolLot/oos:applications/oos:application/oos:applicationParticipants/oos:applicationParticipant/oos:organizationName</t>
+  </si>
+  <si>
+    <t>oos:protocolLots/oos:protocolLot/oos:applications/oos:application/oos:applicationParticipants/oos:applicationParticipant/oos:inn</t>
+  </si>
+  <si>
+    <t>oos:protocolLots/oos:protocolLot/oos:applications/oos:application/oos:applicationParticipants/oos:applicationParticipant/oos:organizationName</t>
+  </si>
+  <si>
+    <t>"2545533"</t>
+  </si>
+  <si>
+    <t>"7726311464"</t>
+  </si>
+  <si>
+    <t>"Закрытое акционерное общество «Р-Фарм»"</t>
+  </si>
+  <si>
+    <t>logical</t>
+  </si>
+  <si>
+    <t>ProtocolLotApplicationJournalNumber</t>
+  </si>
+  <si>
+    <t>ProtocolLotApplicationParticipantINN</t>
+  </si>
+  <si>
+    <t>ProtocolLotApplicationParticipantOrganizationName</t>
+  </si>
+  <si>
+    <t>ProtocolLotApplicationAdmitted</t>
+  </si>
+  <si>
+    <t>ProtocolLotApplicationAppRating</t>
+  </si>
+  <si>
+    <t>/*/d1:contract/oos:singleCustomerReason</t>
+  </si>
+  <si>
+    <t>oos:singleCustomerReason</t>
+  </si>
+  <si>
+    <t>"Point 9 part 2 article 55 - only one bid received"</t>
+  </si>
+  <si>
+    <t>ContractSingleCustomerReason</t>
   </si>
 </sst>
 </file>
@@ -1257,11 +1401,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I65"/>
+  <dimension ref="A1:I83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1718,22 +1862,22 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>290</v>
       </c>
       <c r="D16" t="s">
-        <v>83</v>
+        <v>291</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>39</v>
+        <v>292</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>40</v>
+        <v>293</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>293</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>143</v>
@@ -1747,22 +1891,22 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>143</v>
@@ -1776,22 +1920,22 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>143</v>
@@ -1805,22 +1949,22 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>143</v>
@@ -1834,22 +1978,22 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>143</v>
@@ -1863,25 +2007,25 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>199</v>
+        <v>69</v>
       </c>
       <c r="D21" t="s">
-        <v>200</v>
+        <v>87</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>201</v>
+        <v>50</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>202</v>
+        <v>51</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>202</v>
+        <v>51</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -1892,22 +2036,22 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D22" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>144</v>
@@ -1921,22 +2065,22 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D23" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>144</v>
@@ -1950,22 +2094,22 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D24" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>144</v>
@@ -1979,22 +2123,22 @@
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D25" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>144</v>
@@ -2008,22 +2152,22 @@
         <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>168</v>
+        <v>215</v>
       </c>
       <c r="D26" t="s">
-        <v>169</v>
+        <v>216</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>170</v>
+        <v>217</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>171</v>
+        <v>218</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>171</v>
+        <v>218</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>144</v>
@@ -2037,22 +2181,22 @@
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="D27" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>144</v>
@@ -2066,22 +2210,22 @@
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D28" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>144</v>
@@ -2095,22 +2239,22 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D29" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>144</v>
@@ -2124,22 +2268,22 @@
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>219</v>
+        <v>180</v>
       </c>
       <c r="D30" t="s">
-        <v>220</v>
+        <v>181</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>221</v>
+        <v>182</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>222</v>
+        <v>183</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>222</v>
+        <v>183</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>144</v>
@@ -2153,22 +2297,22 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D31" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>144</v>
@@ -2182,22 +2326,22 @@
         <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D32" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>144</v>
@@ -2211,22 +2355,22 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>184</v>
+        <v>227</v>
       </c>
       <c r="D33" t="s">
-        <v>185</v>
+        <v>228</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>186</v>
+        <v>229</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>187</v>
+        <v>230</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>187</v>
+        <v>230</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>144</v>
@@ -2240,22 +2384,22 @@
         <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D34" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>144</v>
@@ -2269,22 +2413,22 @@
         <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D35" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>31</v>
+        <v>190</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>144</v>
@@ -2298,22 +2442,22 @@
         <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D36" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>197</v>
+        <v>31</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>144</v>
@@ -2327,51 +2471,51 @@
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>231</v>
+        <v>195</v>
       </c>
       <c r="D37" t="s">
-        <v>232</v>
+        <v>196</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>233</v>
+        <v>197</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>234</v>
+        <v>198</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>234</v>
+        <v>198</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>88</v>
+        <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>112</v>
+        <v>231</v>
       </c>
       <c r="D38" t="s">
-        <v>71</v>
+        <v>232</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>90</v>
+        <v>233</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>89</v>
+        <v>234</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>89</v>
+        <v>234</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>143</v>
@@ -2385,22 +2529,22 @@
         <v>88</v>
       </c>
       <c r="C39" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D39" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>5</v>
+        <v>90</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>143</v>
@@ -2414,22 +2558,22 @@
         <v>88</v>
       </c>
       <c r="C40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D40" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>93</v>
+        <v>5</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>143</v>
@@ -2443,22 +2587,22 @@
         <v>88</v>
       </c>
       <c r="C41" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D41" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>143</v>
@@ -2472,22 +2616,22 @@
         <v>88</v>
       </c>
       <c r="C42" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D42" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>143</v>
@@ -2501,22 +2645,22 @@
         <v>88</v>
       </c>
       <c r="C43" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D43" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>143</v>
@@ -2530,22 +2674,22 @@
         <v>88</v>
       </c>
       <c r="C44" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D44" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>143</v>
@@ -2559,22 +2703,22 @@
         <v>88</v>
       </c>
       <c r="C45" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D45" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>143</v>
@@ -2588,22 +2732,22 @@
         <v>88</v>
       </c>
       <c r="C46" t="s">
-        <v>237</v>
+        <v>119</v>
       </c>
       <c r="D46" t="s">
-        <v>238</v>
-      </c>
-      <c r="E46" t="s">
-        <v>239</v>
+        <v>108</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>240</v>
+        <v>110</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>240</v>
+        <v>110</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>143</v>
@@ -2614,28 +2758,28 @@
         <v>88</v>
       </c>
       <c r="B47" t="s">
-        <v>243</v>
+        <v>88</v>
       </c>
       <c r="C47" t="s">
-        <v>128</v>
+        <v>237</v>
       </c>
       <c r="D47" t="s">
-        <v>129</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>93</v>
+        <v>238</v>
+      </c>
+      <c r="E47" t="s">
+        <v>239</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>131</v>
+        <v>240</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>131</v>
+        <v>240</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -2646,22 +2790,22 @@
         <v>243</v>
       </c>
       <c r="C48" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D48" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>134</v>
+        <v>93</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>144</v>
@@ -2675,22 +2819,22 @@
         <v>243</v>
       </c>
       <c r="C49" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="D49" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>37</v>
+        <v>134</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>144</v>
@@ -2701,25 +2845,25 @@
         <v>88</v>
       </c>
       <c r="B50" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C50" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="D50" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>122</v>
+        <v>37</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>144</v>
@@ -2733,22 +2877,22 @@
         <v>244</v>
       </c>
       <c r="C51" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="D51" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="I51" s="1" t="s">
         <v>144</v>
@@ -2759,60 +2903,60 @@
         <v>88</v>
       </c>
       <c r="B52" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C52" t="s">
-        <v>235</v>
+        <v>138</v>
       </c>
       <c r="D52" t="s">
-        <v>236</v>
+        <v>139</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="120" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>88</v>
       </c>
       <c r="B53" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C53" t="s">
-        <v>147</v>
+        <v>235</v>
       </c>
       <c r="D53" t="s">
-        <v>148</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>149</v>
+        <v>236</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="120" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>88</v>
       </c>
@@ -2820,22 +2964,22 @@
         <v>245</v>
       </c>
       <c r="C54" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D54" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>242</v>
+        <v>150</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>144</v>
@@ -2849,28 +2993,28 @@
         <v>245</v>
       </c>
       <c r="C55" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D55" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>158</v>
+        <v>242</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>88</v>
       </c>
@@ -2878,28 +3022,28 @@
         <v>245</v>
       </c>
       <c r="C56" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D56" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="I56" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>88</v>
       </c>
@@ -2907,99 +3051,549 @@
         <v>245</v>
       </c>
       <c r="C57" t="s">
+        <v>159</v>
+      </c>
+      <c r="D57" t="s">
+        <v>160</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H57" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>88</v>
+      </c>
+      <c r="B58" t="s">
+        <v>245</v>
+      </c>
+      <c r="C58" t="s">
         <v>163</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D58" t="s">
         <v>164</v>
       </c>
-      <c r="E57" s="5" t="s">
+      <c r="E58" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F57" s="1" t="s">
+      <c r="F58" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G57" s="1" t="s">
+      <c r="G58" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="H57" s="7" t="s">
+      <c r="H58" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="I57" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="7"/>
+      <c r="I58" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>246</v>
+      </c>
+      <c r="B59" t="s">
+        <v>247</v>
+      </c>
       <c r="C59" t="s">
+        <v>113</v>
+      </c>
+      <c r="D59" t="s">
+        <v>91</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>246</v>
+      </c>
+      <c r="B60" t="s">
+        <v>247</v>
+      </c>
+      <c r="C60" t="s">
+        <v>248</v>
+      </c>
+      <c r="D60" t="s">
+        <v>250</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>246</v>
+      </c>
+      <c r="B61" t="s">
+        <v>247</v>
+      </c>
+      <c r="C61" t="s">
+        <v>249</v>
+      </c>
+      <c r="D61" t="s">
+        <v>251</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>246</v>
+      </c>
+      <c r="B62" t="s">
+        <v>247</v>
+      </c>
+      <c r="C62" t="s">
+        <v>114</v>
+      </c>
+      <c r="D62" t="s">
+        <v>75</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>246</v>
+      </c>
+      <c r="B63" t="s">
+        <v>247</v>
+      </c>
+      <c r="C63" t="s">
+        <v>259</v>
+      </c>
+      <c r="D63" t="s">
+        <v>260</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="H63" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>246</v>
+      </c>
+      <c r="B64" t="s">
+        <v>247</v>
+      </c>
+      <c r="C64" t="s">
+        <v>263</v>
+      </c>
+      <c r="D64" t="s">
+        <v>74</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="H64" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>246</v>
+      </c>
+      <c r="B65" t="s">
+        <v>247</v>
+      </c>
+      <c r="C65" t="s">
+        <v>115</v>
+      </c>
+      <c r="D65" t="s">
+        <v>73</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="H65" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>246</v>
+      </c>
+      <c r="B66" t="s">
+        <v>247</v>
+      </c>
+      <c r="C66" t="s">
+        <v>237</v>
+      </c>
+      <c r="D66" t="s">
+        <v>238</v>
+      </c>
+      <c r="E66" t="s">
+        <v>266</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="H66" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>246</v>
+      </c>
+      <c r="B67" t="s">
+        <v>247</v>
+      </c>
+      <c r="C67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>246</v>
+      </c>
+      <c r="B68" t="s">
+        <v>247</v>
+      </c>
+      <c r="C68" t="s">
+        <v>271</v>
+      </c>
+      <c r="D68" t="s">
+        <v>274</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>246</v>
+      </c>
+      <c r="B69" t="s">
+        <v>247</v>
+      </c>
+      <c r="C69" t="s">
+        <v>277</v>
+      </c>
+      <c r="D69" t="s">
+        <v>279</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>246</v>
+      </c>
+      <c r="B70" t="s">
+        <v>247</v>
+      </c>
+      <c r="C70" t="s">
+        <v>278</v>
+      </c>
+      <c r="D70" t="s">
+        <v>280</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>246</v>
+      </c>
+      <c r="B71" t="s">
+        <v>247</v>
+      </c>
+      <c r="C71" t="s">
+        <v>272</v>
+      </c>
+      <c r="D71" t="s">
+        <v>275</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>246</v>
+      </c>
+      <c r="B72" t="s">
+        <v>247</v>
+      </c>
+      <c r="C72" t="s">
+        <v>273</v>
+      </c>
+      <c r="D72" t="s">
+        <v>276</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="7"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="7"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="7"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="7"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="7"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="7"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C79" t="s">
         <v>111</v>
       </c>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-      <c r="H59" s="7"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-      <c r="H60" s="7"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H61" s="7"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B62" t="s">
+      <c r="H79" s="7"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B80" t="s">
         <v>43</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C80" t="s">
         <v>44</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="E80" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F62" s="1" t="s">
+      <c r="F80" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G62" s="1" t="s">
+      <c r="G80" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H62" s="7" t="s">
+      <c r="H80" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B63" t="s">
-        <v>2</v>
-      </c>
-      <c r="C63" t="s">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B81" t="s">
+        <v>2</v>
+      </c>
+      <c r="C81" t="s">
         <v>57</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="E81" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F63" s="1" t="s">
+      <c r="F81" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G63" s="1" t="s">
+      <c r="G81" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H63" s="7" t="s">
+      <c r="H81" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H64" s="7"/>
-    </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B65" t="s">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="H82" s="7"/>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B83" t="s">
         <v>103</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C83" t="s">
         <v>104</v>
       </c>
-      <c r="H65" s="7"/>
+      <c r="H83" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adjusting cleaner to be as aggressive as previously in discarding contracts
</commit_message>
<xml_diff>
--- a/3-Unpack/how-I-parse-the-xml.xlsx
+++ b/3-Unpack/how-I-parse-the-xml.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27106"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/shaun/git/shaun-mcgirr-dissertation/3-Unpack/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaun/git/shaun-mcgirr-dissertation/3-Unpack/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -59,6 +59,33 @@
         </r>
       </text>
     </comment>
+    <comment ref="E38" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Options are
+&lt;xs:documentation&gt;Текущее состояние контракта:
+E  Исполнение;
+ET Исполнение прекращено;
+EC Исполнение завершено;
+IN Aннулировано.&lt;/xs:documentation&gt;</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -955,7 +982,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1014,6 +1041,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1405,7 +1443,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Starting to add ability to parse protocols for number of bidders
</commit_message>
<xml_diff>
--- a/3-Unpack/how-I-parse-the-xml.xlsx
+++ b/3-Unpack/how-I-parse-the-xml.xlsx
@@ -32,6 +32,28 @@
     <author>Author</author>
   </authors>
   <commentList>
+    <comment ref="C2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Identifier of document must be first field, version third</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C4" authorId="0">
       <text>
         <r>
@@ -83,6 +105,28 @@
 ET Исполнение прекращено;
 EC Исполнение завершено;
 IN Aннулировано.&lt;/xs:documentation&gt;</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C61" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Must be third in list</t>
         </r>
       </text>
     </comment>
@@ -1442,8 +1486,8 @@
   <dimension ref="A1:I83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3147,22 +3191,22 @@
         <v>247</v>
       </c>
       <c r="C59" t="s">
-        <v>113</v>
+        <v>248</v>
       </c>
       <c r="D59" t="s">
-        <v>91</v>
+        <v>250</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>143</v>
@@ -3176,22 +3220,22 @@
         <v>247</v>
       </c>
       <c r="C60" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D60" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="I60" s="1" t="s">
         <v>143</v>
@@ -3205,25 +3249,25 @@
         <v>247</v>
       </c>
       <c r="C61" t="s">
-        <v>249</v>
+        <v>114</v>
       </c>
       <c r="D61" t="s">
-        <v>251</v>
+        <v>75</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>254</v>
+        <v>93</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
@@ -3234,25 +3278,25 @@
         <v>247</v>
       </c>
       <c r="C62" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D62" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>93</v>
+        <v>252</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>